<commit_message>
chore: change accessor to support formula in excel
</commit_message>
<xml_diff>
--- a/src/test/resources/formula-excel.xlsx
+++ b/src/test/resources/formula-excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ysgao/Projects/me/persistence-excel/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49BD6BA5-EB49-6F4D-863F-BFCFCDAE3B4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F53386C-C4DC-8546-AE2C-F3BE88FAF926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{C0E8BB31-93EB-1E44-80E4-4D4D327F606C}"/>
+    <workbookView xWindow="9620" yWindow="9060" windowWidth="27640" windowHeight="16940" xr2:uid="{C0E8BB31-93EB-1E44-80E4-4D4D327F606C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
     <t>Favorite Date</t>
   </si>
   <si>
-    <t>Tom</t>
+    <t>Remark</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -434,10 +434,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>5</v>
+      <c r="A2" t="str">
+        <f>CONCATENATE(F1,"_",F2)</f>
+        <v>Remark_12</v>
       </c>
       <c r="B2">
         <f>F2+G2</f>

</xml_diff>